<commit_message>
# Conflicts: #	src/main/java/com/tpay/domains/vat/application/VatHomeTaxService.java
</commit_message>
<xml_diff>
--- a/src/main/resources/KTP_CMS_Form.xlsx
+++ b/src/main/resources/KTP_CMS_Form.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/backend/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/backend/sdk/tpay-server/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E338AB-FD6D-CE42-9E5A-CB6ACD8A2502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE06755B-EA76-384F-8175-A9660C0F92D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8120" yWindow="3160" windowWidth="33700" windowHeight="23520" xr2:uid="{5F7638EB-4457-4D6A-A575-6A1299AB4C0E}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{5F7638EB-4457-4D6A-A575-6A1299AB4C0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$56</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$93</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$A$1:$J$57</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -318,7 +318,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -359,6 +359,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -387,15 +413,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -405,32 +425,23 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
@@ -441,22 +452,37 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -480,16 +506,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -535,13 +561,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>322729</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>114551</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>779832</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>92</xdr:row>
       <xdr:rowOff>55166</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -881,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC6348C-D3DF-438B-B808-4FA430F3AD7D}">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A50" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H78" sqref="H78:I78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -900,7 +926,7 @@
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="3.5" customHeight="1">
       <c r="A4" s="1"/>
@@ -925,22 +951,22 @@
     </row>
     <row r="8" spans="1:10" ht="18.5" customHeight="1"/>
     <row r="9" spans="1:10">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="11" t="s">
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10">
       <c r="B10" s="6"/>
@@ -954,16 +980,16 @@
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
     </row>
@@ -980,7 +1006,7 @@
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="5"/>
@@ -1006,18 +1032,18 @@
       <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10" ht="5.5" customHeight="1"/>
     <row r="17" spans="1:10" ht="5.5" customHeight="1">
@@ -1060,26 +1086,26 @@
       <c r="J20" s="37"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
     </row>
     <row r="23" spans="1:10" ht="44.5" customHeight="1">
       <c r="A23" s="38"/>
@@ -1094,7 +1120,7 @@
       <c r="J23" s="38"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="C24" s="15"/>
+      <c r="C24" s="11"/>
     </row>
     <row r="25" spans="1:10" ht="19.25" customHeight="1">
       <c r="B25" s="39" t="s">
@@ -1109,7 +1135,7 @@
       <c r="G25" s="39"/>
       <c r="H25" s="41"/>
       <c r="I25" s="41"/>
-      <c r="J25" s="17"/>
+      <c r="J25" s="13"/>
     </row>
     <row r="26" spans="1:10" ht="17.5" customHeight="1">
       <c r="B26" s="40"/>
@@ -1122,30 +1148,29 @@
       <c r="I26" s="42"/>
     </row>
     <row r="27" spans="1:10" ht="17.5" customHeight="1">
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="J29" s="7"/>
+      <c r="B29" s="11"/>
+      <c r="J29" s="6"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="33" t="s">
@@ -1164,246 +1189,721 @@
         <v>8</v>
       </c>
       <c r="I30" s="33"/>
-      <c r="J30" s="24" t="s">
+      <c r="J30" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="20"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="21"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="17"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="20"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="21"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="17"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="20"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="21"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="17"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="20"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="21"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="17"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="20"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="21"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="17"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="20"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="21"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="17"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="20"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="28"/>
-      <c r="J37" s="21"/>
+      <c r="A37" s="16"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="17"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="20"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="28"/>
-      <c r="J38" s="21"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="17"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="20"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="28"/>
-      <c r="J39" s="21"/>
+      <c r="A39" s="16"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="17"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="20"/>
-      <c r="B40" s="28"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="28"/>
-      <c r="J40" s="21"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="17"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="20"/>
-      <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="28"/>
-      <c r="I41" s="28"/>
-      <c r="J41" s="21"/>
+      <c r="A41" s="16"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="17"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="20"/>
-      <c r="B42" s="28"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="30"/>
-      <c r="G42" s="30"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="21"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
+      <c r="J42" s="17"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="20"/>
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="30"/>
-      <c r="G43" s="30"/>
-      <c r="H43" s="28"/>
-      <c r="I43" s="28"/>
-      <c r="J43" s="21"/>
+      <c r="A43" s="16"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="17"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="20"/>
-      <c r="B44" s="28"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="30"/>
-      <c r="G44" s="30"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="28"/>
-      <c r="J44" s="21"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="17"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="20"/>
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="30"/>
-      <c r="G45" s="30"/>
-      <c r="H45" s="28"/>
-      <c r="I45" s="28"/>
-      <c r="J45" s="21"/>
-    </row>
-    <row r="46" spans="1:10" ht="42" customHeight="1">
-      <c r="A46" s="20">
+      <c r="A45" s="16"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="17"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="16"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="17"/>
+    </row>
+    <row r="47" spans="1:10" ht="17" customHeight="1">
+      <c r="A47" s="16"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="23"/>
+      <c r="I47" s="23"/>
+      <c r="J47" s="17"/>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="16"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
+      <c r="J48" s="17"/>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="16"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="17"/>
+    </row>
+    <row r="50" spans="1:10" ht="17" customHeight="1">
+      <c r="A50" s="16"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="23"/>
+      <c r="I50" s="23"/>
+      <c r="J50" s="17"/>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="16"/>
+      <c r="B51" s="23"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="23"/>
+      <c r="I51" s="23"/>
+      <c r="J51" s="17"/>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="16"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="23"/>
+      <c r="I52" s="23"/>
+      <c r="J52" s="17"/>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="16"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="23"/>
+      <c r="I53" s="23"/>
+      <c r="J53" s="17"/>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="16"/>
+      <c r="B54" s="23"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="23"/>
+      <c r="I54" s="23"/>
+      <c r="J54" s="17"/>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="16"/>
+      <c r="B55" s="23"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="22"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="23"/>
+      <c r="I55" s="23"/>
+      <c r="J55" s="17"/>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="16"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="22"/>
+      <c r="G56" s="22"/>
+      <c r="H56" s="23"/>
+      <c r="I56" s="23"/>
+      <c r="J56" s="17"/>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="16"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="22"/>
+      <c r="G57" s="22"/>
+      <c r="H57" s="23"/>
+      <c r="I57" s="23"/>
+      <c r="J57" s="17"/>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="16"/>
+      <c r="B58" s="29"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="28"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="23"/>
+      <c r="I58" s="23"/>
+      <c r="J58" s="17"/>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="16"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="22"/>
+      <c r="G59" s="22"/>
+      <c r="H59" s="23"/>
+      <c r="I59" s="23"/>
+      <c r="J59" s="17"/>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="16"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="22"/>
+      <c r="G60" s="22"/>
+      <c r="H60" s="23"/>
+      <c r="I60" s="23"/>
+      <c r="J60" s="17"/>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="16"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="24"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="22"/>
+      <c r="G61" s="22"/>
+      <c r="H61" s="23"/>
+      <c r="I61" s="23"/>
+      <c r="J61" s="17"/>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" s="16"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="22"/>
+      <c r="G62" s="22"/>
+      <c r="H62" s="23"/>
+      <c r="I62" s="23"/>
+      <c r="J62" s="17"/>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="16"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="22"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="23"/>
+      <c r="I63" s="23"/>
+      <c r="J63" s="17"/>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="16"/>
+      <c r="B64" s="23"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="24"/>
+      <c r="F64" s="22"/>
+      <c r="G64" s="22"/>
+      <c r="H64" s="23"/>
+      <c r="I64" s="23"/>
+      <c r="J64" s="17"/>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" s="16"/>
+      <c r="B65" s="23"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="24"/>
+      <c r="E65" s="24"/>
+      <c r="F65" s="22"/>
+      <c r="G65" s="22"/>
+      <c r="H65" s="23"/>
+      <c r="I65" s="23"/>
+      <c r="J65" s="17"/>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="16"/>
+      <c r="B66" s="23"/>
+      <c r="C66" s="23"/>
+      <c r="D66" s="24"/>
+      <c r="E66" s="24"/>
+      <c r="F66" s="22"/>
+      <c r="G66" s="22"/>
+      <c r="H66" s="23"/>
+      <c r="I66" s="23"/>
+      <c r="J66" s="17"/>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="16"/>
+      <c r="B67" s="23"/>
+      <c r="C67" s="23"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="22"/>
+      <c r="G67" s="22"/>
+      <c r="H67" s="23"/>
+      <c r="I67" s="23"/>
+      <c r="J67" s="17"/>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="16"/>
+      <c r="B68" s="23"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="24"/>
+      <c r="F68" s="22"/>
+      <c r="G68" s="22"/>
+      <c r="H68" s="23"/>
+      <c r="I68" s="23"/>
+      <c r="J68" s="17"/>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="16"/>
+      <c r="B69" s="23"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="24"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="22"/>
+      <c r="G69" s="22"/>
+      <c r="H69" s="23"/>
+      <c r="I69" s="23"/>
+      <c r="J69" s="17"/>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="16"/>
+      <c r="B70" s="23"/>
+      <c r="C70" s="23"/>
+      <c r="D70" s="24"/>
+      <c r="E70" s="24"/>
+      <c r="F70" s="22"/>
+      <c r="G70" s="22"/>
+      <c r="H70" s="23"/>
+      <c r="I70" s="23"/>
+      <c r="J70" s="17"/>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="16"/>
+      <c r="B71" s="23"/>
+      <c r="C71" s="23"/>
+      <c r="D71" s="24"/>
+      <c r="E71" s="24"/>
+      <c r="F71" s="22"/>
+      <c r="G71" s="22"/>
+      <c r="H71" s="23"/>
+      <c r="I71" s="23"/>
+      <c r="J71" s="17"/>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="16"/>
+      <c r="B72" s="23"/>
+      <c r="C72" s="23"/>
+      <c r="D72" s="24"/>
+      <c r="E72" s="24"/>
+      <c r="F72" s="22"/>
+      <c r="G72" s="22"/>
+      <c r="H72" s="23"/>
+      <c r="I72" s="23"/>
+      <c r="J72" s="17"/>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="16"/>
+      <c r="B73" s="23"/>
+      <c r="C73" s="23"/>
+      <c r="D73" s="24"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="22"/>
+      <c r="G73" s="22"/>
+      <c r="H73" s="23"/>
+      <c r="I73" s="23"/>
+      <c r="J73" s="17"/>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" s="16"/>
+      <c r="B74" s="23"/>
+      <c r="C74" s="23"/>
+      <c r="D74" s="24"/>
+      <c r="E74" s="24"/>
+      <c r="F74" s="22"/>
+      <c r="G74" s="22"/>
+      <c r="H74" s="23"/>
+      <c r="I74" s="23"/>
+      <c r="J74" s="17"/>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="16"/>
+      <c r="B75" s="23"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="24"/>
+      <c r="E75" s="24"/>
+      <c r="F75" s="22"/>
+      <c r="G75" s="22"/>
+      <c r="H75" s="23"/>
+      <c r="I75" s="23"/>
+      <c r="J75" s="17"/>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" s="16"/>
+      <c r="B76" s="29"/>
+      <c r="C76" s="30"/>
+      <c r="D76" s="27"/>
+      <c r="E76" s="28"/>
+      <c r="F76" s="25"/>
+      <c r="G76" s="26"/>
+      <c r="H76" s="29"/>
+      <c r="I76" s="30"/>
+      <c r="J76" s="17"/>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="16"/>
+      <c r="B77" s="29"/>
+      <c r="C77" s="30"/>
+      <c r="D77" s="27"/>
+      <c r="E77" s="28"/>
+      <c r="F77" s="25"/>
+      <c r="G77" s="26"/>
+      <c r="H77" s="29"/>
+      <c r="I77" s="30"/>
+      <c r="J77" s="17"/>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="16"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="30"/>
+      <c r="D78" s="27"/>
+      <c r="E78" s="28"/>
+      <c r="F78" s="25"/>
+      <c r="G78" s="26"/>
+      <c r="H78" s="29"/>
+      <c r="I78" s="30"/>
+      <c r="J78" s="17"/>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="16"/>
+      <c r="B79" s="29"/>
+      <c r="C79" s="30"/>
+      <c r="D79" s="27"/>
+      <c r="E79" s="28"/>
+      <c r="F79" s="25"/>
+      <c r="G79" s="26"/>
+      <c r="H79" s="29"/>
+      <c r="I79" s="30"/>
+      <c r="J79" s="17"/>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="B80" s="29"/>
+      <c r="C80" s="30"/>
+      <c r="D80" s="27"/>
+      <c r="E80" s="28"/>
+      <c r="F80" s="25"/>
+      <c r="G80" s="26"/>
+      <c r="H80" s="29"/>
+      <c r="I80" s="30"/>
+      <c r="J80" s="17"/>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" s="16"/>
+      <c r="B81" s="29"/>
+      <c r="C81" s="30"/>
+      <c r="D81" s="27"/>
+      <c r="E81" s="28"/>
+      <c r="F81" s="25"/>
+      <c r="G81" s="26"/>
+      <c r="H81" s="29"/>
+      <c r="I81" s="30"/>
+      <c r="J81" s="17"/>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" s="16"/>
+      <c r="B82" s="23"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="24"/>
+      <c r="E82" s="24"/>
+      <c r="F82" s="22"/>
+      <c r="G82" s="22"/>
+      <c r="H82" s="23"/>
+      <c r="I82" s="23"/>
+      <c r="J82" s="17"/>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83" s="16"/>
+      <c r="B83" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B46" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="31"/>
-      <c r="I46" s="31"/>
-      <c r="J46" s="22"/>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="13" t="s">
+      <c r="C83" s="32"/>
+      <c r="D83" s="32"/>
+      <c r="E83" s="32"/>
+      <c r="F83" s="31"/>
+      <c r="G83" s="31"/>
+      <c r="H83" s="31"/>
+      <c r="I83" s="31"/>
+      <c r="J83" s="17"/>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="29.5" customHeight="1">
-      <c r="A49" s="34" t="s">
+    <row r="86" spans="1:10">
+      <c r="A86" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B49" s="34"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="34"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="34"/>
-      <c r="H49" s="34"/>
-      <c r="I49" s="34"/>
-      <c r="J49" s="34"/>
-    </row>
-    <row r="52" spans="1:10">
-      <c r="F52" s="35" t="s">
+      <c r="B86" s="34"/>
+      <c r="C86" s="34"/>
+      <c r="D86" s="34"/>
+      <c r="E86" s="34"/>
+      <c r="F86" s="34"/>
+      <c r="G86" s="34"/>
+      <c r="H86" s="34"/>
+      <c r="I86" s="34"/>
+      <c r="J86" s="34"/>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="F89" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="G52" s="35"/>
-      <c r="H52" s="35"/>
-      <c r="I52" s="9"/>
-    </row>
-    <row r="53" spans="1:10">
-      <c r="F53" s="35" t="s">
+      <c r="G89" s="35"/>
+      <c r="H89" s="35"/>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="F90" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="G53" s="35"/>
-      <c r="H53" s="35"/>
-      <c r="I53" s="9"/>
+      <c r="G90" s="35"/>
+      <c r="H90" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="77">
-    <mergeCell ref="A49:J49"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F53:H53"/>
+  <mergeCells count="225">
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="H68:I68"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="A86:J86"/>
+    <mergeCell ref="F89:H89"/>
+    <mergeCell ref="F90:H90"/>
     <mergeCell ref="D13:H13"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="D32:E32"/>
@@ -1417,67 +1917,179 @@
     <mergeCell ref="D25:E26"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
     <mergeCell ref="F30:G30"/>
     <mergeCell ref="H30:I30"/>
     <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="F33:G33"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="B34:C34"/>
     <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="B36:C36"/>
     <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="H78:I78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="H79:I79"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="F78:G78"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="H82:I82"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="H83:I83"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
     <mergeCell ref="H39:I39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="F39:G39"/>
     <mergeCell ref="F40:G40"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
     <mergeCell ref="F38:G38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="B46:E46"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1507,7 +2119,7 @@
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="3.5" customHeight="1">
       <c r="A4" s="1"/>
@@ -1532,7 +2144,7 @@
     </row>
     <row r="8" spans="1:10" ht="18.5" customHeight="1"/>
     <row r="9" spans="1:10">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="6"/>
@@ -1540,10 +2152,10 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="25"/>
+      <c r="H9" s="14"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
@@ -1559,7 +2171,7 @@
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="6"/>
@@ -1585,7 +2197,7 @@
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="5"/>
@@ -1611,7 +2223,7 @@
       <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="6"/>
@@ -1665,14 +2277,14 @@
       <c r="J20" s="37"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="15"/>
+      <c r="B21" s="11"/>
       <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="45" t="s">
@@ -1691,12 +2303,12 @@
         <v>8</v>
       </c>
       <c r="I22" s="46"/>
-      <c r="J22" s="27" t="s">
+      <c r="J22" s="21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="19"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="34"/>
       <c r="C23" s="34"/>
       <c r="D23" s="43"/>
@@ -1707,7 +2319,7 @@
       <c r="I23" s="34"/>
     </row>
     <row r="24" spans="1:10" ht="19.25" customHeight="1">
-      <c r="A24" s="19"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="34"/>
       <c r="C24" s="34"/>
       <c r="D24" s="43"/>
@@ -1718,7 +2330,7 @@
       <c r="I24" s="34"/>
     </row>
     <row r="25" spans="1:10" ht="17.5" customHeight="1">
-      <c r="A25" s="19"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="34"/>
       <c r="C25" s="34"/>
       <c r="D25" s="43"/>
@@ -1729,7 +2341,7 @@
       <c r="I25" s="34"/>
     </row>
     <row r="26" spans="1:10" ht="17.5" customHeight="1">
-      <c r="A26" s="19"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="34"/>
       <c r="C26" s="34"/>
       <c r="D26" s="43"/>
@@ -1740,7 +2352,7 @@
       <c r="I26" s="34"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="19"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="34"/>
       <c r="C27" s="34"/>
       <c r="D27" s="43"/>
@@ -1751,7 +2363,7 @@
       <c r="I27" s="34"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="19"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="34"/>
       <c r="C28" s="34"/>
       <c r="D28" s="43"/>
@@ -1762,7 +2374,7 @@
       <c r="I28" s="34"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="19"/>
+      <c r="A29" s="15"/>
       <c r="B29" s="34"/>
       <c r="C29" s="34"/>
       <c r="D29" s="43"/>
@@ -1773,7 +2385,7 @@
       <c r="I29" s="34"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="19"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="34"/>
       <c r="C30" s="34"/>
       <c r="D30" s="43"/>
@@ -1784,7 +2396,7 @@
       <c r="I30" s="34"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="19"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="34"/>
       <c r="C31" s="34"/>
       <c r="D31" s="43"/>
@@ -1795,7 +2407,7 @@
       <c r="I31" s="34"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="19"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="34"/>
       <c r="C32" s="34"/>
       <c r="D32" s="43"/>
@@ -1806,7 +2418,7 @@
       <c r="I32" s="34"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="19"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="34"/>
       <c r="C33" s="34"/>
       <c r="D33" s="43"/>
@@ -1817,7 +2429,7 @@
       <c r="I33" s="34"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="19"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="34"/>
       <c r="C34" s="34"/>
       <c r="D34" s="43"/>
@@ -1828,7 +2440,7 @@
       <c r="I34" s="34"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="19"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="34"/>
       <c r="C35" s="34"/>
       <c r="D35" s="43"/>
@@ -1839,7 +2451,7 @@
       <c r="I35" s="34"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="19"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="34"/>
       <c r="C36" s="34"/>
       <c r="D36" s="43"/>
@@ -1850,7 +2462,7 @@
       <c r="I36" s="34"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="19"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="34"/>
       <c r="C37" s="34"/>
       <c r="D37" s="43"/>

</xml_diff>